<commit_message>
Fix: test file 수정
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -478,22 +478,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[11, 41, 78, 114, 207, 249, 371, 364, 454, 504, 677, 759, 902]</t>
+          <t>[11, 35, 78, 123, 167, 246, 281, 366, 502, 609, 715, 755, 859]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[17, 66, 125, 216, 370, 546, 755, 955, 1203, 1485, 1961, 2243, 2711]</t>
+          <t>[17, 57, 136, 248, 356, 514, 766, 918, 1362, 1516, 2005, 2325, 2737]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[2, 9, 18, 32, 57, 87, 122, 156, 198, 242, 315, 360, 449]</t>
+          <t>[2, 9, 21, 38, 54, 81, 125, 150, 228, 248, 318, 393, 455]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[0.9333855344173657, 0.952730021995015, 0.9071720822833819, 0.8399189000564958, 0.7197061072504335, 0.6124854072427482, 0.4817372742918409, 0.3786945269960076, 0.2827982092804997, 0.22235954711186245, 0.13627711515933344, 0.09562388260002992, 0.05555291759746782]</t>
+          <t>[0.9333855344173657, 0.9546379362064165, 0.9035434077349098, 0.8053226360366034, 0.7249619150987372, 0.604319875930438, 0.5088548272825192, 0.3850235746730784, 0.24498917805420162, 0.21848481890473787, 0.11590220413675477, 0.08661139797050864, 0.05278898009786382]</t>
         </is>
       </c>
     </row>
@@ -510,22 +510,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[12, 38, 75, 106, 169, 233, 295, 330, 464, 404, 465, 643, 736]</t>
+          <t>[12, 41, 74, 103, 144, 234, 271, 299, 367, 465, 519, 582, 737]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[14, 57, 105, 158, 266, 414, 604, 733, 1046, 1115, 1321, 1701, 2176]</t>
+          <t>[14, 56, 105, 158, 258, 407, 585, 704, 952, 1251, 1448, 1670, 2059]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[2, 9, 18, 30, 50, 73, 108, 132, 185, 186, 234, 312, 373]</t>
+          <t>[2, 9, 18, 30, 46, 73, 103, 117, 160, 217, 249, 295, 366]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[0.9907223290650904, 0.9570525968091622, 0.9088024428860046, 0.8535009160150564, 0.7690643634907555, 0.657985202335546, 0.5383131744434865, 0.4709699496901323, 0.3187126910234874, 0.3209533909524098, 0.23280989660660098, 0.14228287892136063, 0.08829375524573659]</t>
+          <t>[0.9918619131687658, 0.9569862094315925, 0.9092902045510506, 0.8470297967650031, 0.762929690000467, 0.6367971673481913, 0.5405187714385588, 0.49981810825897294, 0.397799615523347, 0.2642867237873717, 0.2130036236066909, 0.1456252319645504, 0.08849984908031076]</t>
         </is>
       </c>
     </row>
@@ -542,22 +542,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[12, 36, 75, 110, 169, 208, 234, 300, 426, 493, 645, 553, 614]</t>
+          <t>[12, 41, 74, 109, 145, 213, 257, 337, 432, 537, 505, 718, 819]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[14, 49, 105, 175, 265, 380, 537, 708, 946, 1213, 1544, 1783, 2243]</t>
+          <t>[14, 56, 105, 171, 256, 392, 538, 744, 931, 1242, 1374, 1873, 2217]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[2, 9, 18, 30, 50, 70, 91, 120, 167, 225, 281, 313, 410]</t>
+          <t>[2, 9, 18, 30, 46, 70, 91, 132, 167, 228, 233, 339, 407]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[0.9908555768363504, 0.9573593763480913, 0.9088024428860046, 0.8523377656254297, 0.7690643634907555, 0.6853020544400216, 0.5888403859205847, 0.5039179778509593, 0.36585792646421855, 0.2713074512332678, 0.18037413492668053, 0.16850192261538532, 0.08150664251366987]</t>
+          <t>[0.9918619131687658, 0.9569862094315925, 0.9092902045510506, 0.8440360490253149, 0.7630999303838633, 0.6661534780293442, 0.5925685280846694, 0.44554571349759303, 0.3454116342015505, 0.2567005389107025, 0.23662510018397004, 0.12186712833352296, 0.06928845650696905]</t>
         </is>
       </c>
     </row>
@@ -574,22 +574,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[12, 33, 60, 100, 119, 143, 168, 205, 283, 283, 333, 415, 448]</t>
+          <t>[12, 33, 61, 85, 119, 144, 193, 225, 255, 247, 320, 401, 371]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[14, 46, 106, 200, 272, 399, 546, 721, 922, 1111, 1433, 1595, 1964]</t>
+          <t>[14, 47, 89, 175, 272, 392, 558, 727, 927, 1094, 1385, 1663, 1849]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[2, 7, 16, 31, 43, 61, 82, 108, 148, 169, 222, 256, 311]</t>
+          <t>[2, 7, 14, 27, 43, 61, 90, 114, 144, 163, 211, 260, 284]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[0.9341209303613215, 0.9636247560715911, 0.8464062590530965, 0.8115730552996565, 0.6236842479730242, 0.7087782830532328, 0.0, 0.0, 0.31493336112563264, 0.2568180108222445, 0.0, 0.0, 0.0]</t>
+          <t>[0.9341209303613215, 0.9595201151698435, 0.8370982389394316, 0.0, 0.7674899632460251, 0.6547107510348122, 0.39575427674543545, 0.4949941536587924, 0.3819051447804764, 0.2711603684251308, 0.23896966769282196, 0.0, 0.1451274985063912]</t>
         </is>
       </c>
     </row>

</xml_diff>